<commit_message>
More images, fixes on products page
</commit_message>
<xml_diff>
--- a/static/products.xlsx
+++ b/static/products.xlsx
@@ -8,28 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garya\Documents\0_ckpublic\ckpublic\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B445A696-33E7-4629-BDC3-4F7E4FAE20D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F522BD-5744-415C-8BCC-DE31818512DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="3" xr2:uid="{291B890B-F5D5-4F8E-937E-5F9F8EBD0536}"/>
+    <workbookView xWindow="4850" yWindow="0" windowWidth="16800" windowHeight="9760" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Signature" sheetId="4" r:id="rId1"/>
-    <sheet name="Products" sheetId="1" r:id="rId2"/>
-    <sheet name="Hampers" sheetId="2" r:id="rId3"/>
-    <sheet name="Snacks" sheetId="3" r:id="rId4"/>
+    <sheet name="Signature" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" r:id="rId2"/>
+    <sheet name="Hampers" sheetId="3" r:id="rId3"/>
+    <sheet name="Snacks" sheetId="4" r:id="rId4"/>
     <sheet name="Checklist" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Common Price</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
   <si>
     <t>Nastar</t>
   </si>
@@ -40,16 +44,13 @@
     <t>Sagu Keju</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Nanas</t>
-  </si>
-  <si>
-    <t>Common Price</t>
+    <t>Kenari Coklat</t>
+  </si>
+  <si>
+    <t>Putri Salju</t>
+  </si>
+  <si>
+    <t>Kenari Cookies</t>
   </si>
   <si>
     <t>Nastar Keju</t>
@@ -79,12 +80,6 @@
     <t>Sagu Coklat</t>
   </si>
   <si>
-    <t>Kenari Cookies</t>
-  </si>
-  <si>
-    <t>Kenari Coklat</t>
-  </si>
-  <si>
     <t>Choco Cheese</t>
   </si>
   <si>
@@ -103,18 +98,12 @@
     <t>Butter Cookies Coklat</t>
   </si>
   <si>
-    <t>Putri Salju</t>
-  </si>
-  <si>
     <t>Peanut Cookies</t>
   </si>
   <si>
     <t>Nastar Garis</t>
   </si>
   <si>
-    <t>Lidah Kucing</t>
-  </si>
-  <si>
     <t>Santa Claus Bag</t>
   </si>
   <si>
@@ -124,7 +113,7 @@
     <t>Round Bag</t>
   </si>
   <si>
-    <t>Premium Red</t>
+    <t>Premium Red Box</t>
   </si>
   <si>
     <t>Premium Small Box</t>
@@ -145,13 +134,13 @@
     <t>Red Basket Gold</t>
   </si>
   <si>
-    <t>Premium Red Basket Diamond</t>
-  </si>
-  <si>
-    <t>Premium Red Basket Sapphire</t>
-  </si>
-  <si>
-    <t>Premium Red Basket Emerald</t>
+    <t>Red Basket Diamond</t>
+  </si>
+  <si>
+    <t>Red Basket Sapphire</t>
+  </si>
+  <si>
+    <t>Red Basket Emerald</t>
   </si>
   <si>
     <t>Parcel Rangkai A</t>
@@ -169,12 +158,18 @@
     <t>Jumbo Box B</t>
   </si>
   <si>
+    <t>Premium Bag A</t>
+  </si>
+  <si>
+    <t>Premium Bag B</t>
+  </si>
+  <si>
+    <t>Soesring Tabung Original</t>
+  </si>
+  <si>
     <t>Soesring Tabung Coklat</t>
   </si>
   <si>
-    <t>Soesring Tabung Original</t>
-  </si>
-  <si>
     <t>Soesring Pouch Original</t>
   </si>
   <si>
@@ -202,22 +197,10 @@
     <t>Almond Disc Cheese</t>
   </si>
   <si>
-    <t>Premium Red Box</t>
-  </si>
-  <si>
-    <t>Red Basket Diamond</t>
-  </si>
-  <si>
-    <t>Red Basket Sapphire</t>
-  </si>
-  <si>
-    <t>Red Basket Emerald</t>
-  </si>
-  <si>
-    <t>Premium Bag A</t>
-  </si>
-  <si>
-    <t>Premium Bag B</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -586,11 +569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8673F4E-76D8-41D3-857E-5AB6E750EB09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,18 +586,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>78000</v>
@@ -622,7 +605,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>115000</v>
@@ -630,7 +613,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>62000</v>
@@ -638,7 +621,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>73000</v>
@@ -646,7 +629,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>73000</v>
@@ -654,7 +637,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>55000</v>
@@ -662,7 +645,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>73000</v>
@@ -674,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB413927-E9F9-4C56-ACF5-DA02F92C04DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,29 +674,26 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>78000</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>78000</v>
@@ -721,7 +701,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>105000</v>
@@ -729,7 +709,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>115000</v>
@@ -737,7 +717,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>73000</v>
@@ -745,7 +725,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>73000</v>
@@ -753,7 +733,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>78000</v>
@@ -761,7 +741,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>78000</v>
@@ -769,7 +749,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
         <v>115000</v>
@@ -777,7 +757,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>62000</v>
@@ -785,7 +765,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>62000</v>
@@ -793,7 +773,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
         <v>62000</v>
@@ -801,7 +781,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>73000</v>
@@ -809,7 +789,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2">
         <v>730000</v>
@@ -865,7 +845,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2">
         <v>55000</v>
@@ -873,7 +853,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2">
         <v>60000</v>
@@ -881,7 +861,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2">
         <v>60000</v>
@@ -889,16 +869,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48B4025-030B-428D-AF05-C3C9A37A8DAC}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,13 +891,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -925,7 +905,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="2">
-        <v>80000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -933,7 +913,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2">
-        <v>145000</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -941,15 +921,15 @@
         <v>30</v>
       </c>
       <c r="B4" s="2">
-        <v>150000</v>
+        <v>205000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2">
-        <v>180000</v>
+        <v>265000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -957,7 +937,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="2">
-        <v>205000</v>
+        <v>340000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -965,7 +945,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="2">
-        <v>265000</v>
+        <v>440000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -973,7 +953,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="2">
-        <v>340000</v>
+        <v>540000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -981,7 +961,7 @@
         <v>35</v>
       </c>
       <c r="B9" s="2">
-        <v>440000</v>
+        <v>640000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -989,7 +969,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="2">
-        <v>540000</v>
+        <v>620000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -997,31 +977,31 @@
         <v>37</v>
       </c>
       <c r="B11" s="2">
-        <v>640000</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2">
-        <v>620000</v>
+        <v>920000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2">
-        <v>720000</v>
+        <v>730000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2">
-        <v>920000</v>
+        <v>930000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1029,7 +1009,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="2">
-        <v>730000</v>
+        <v>1130000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1037,7 +1017,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="2">
-        <v>930000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1045,7 +1025,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="2">
-        <v>1130000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1053,7 +1033,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="2">
-        <v>400000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1061,31 +1041,7 @@
         <v>45</v>
       </c>
       <c r="B19" s="2">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="2">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="2">
         <v>330000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="2">
-        <v>150000</v>
       </c>
     </row>
   </sheetData>
@@ -1094,11 +1050,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A673D553-35C1-46D3-B8E0-0A33C52880A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1111,18 +1067,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2">
         <v>21000</v>
@@ -1130,7 +1086,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2">
         <v>29000</v>
@@ -1214,11 +1170,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB501936-94A8-482C-A6A6-EFAE123CCEF7}">
-  <dimension ref="A1:A47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:A47"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1226,238 +1182,317 @@
     <col min="1" max="1" width="33.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B27">
+        <v>8762</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B28">
+        <v>8794</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B30">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44">
+        <v>8778</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Products Fix, Certifications, Locations
</commit_message>
<xml_diff>
--- a/static/products.xlsx
+++ b/static/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garya\Documents\0_ckpublic\ckpublic\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F522BD-5744-415C-8BCC-DE31818512DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D579A3-9505-418D-9B73-A95CD1D63ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4850" yWindow="0" windowWidth="16800" windowHeight="9760" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signature" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -65,21 +65,12 @@
     <t>Lidah Kucing Original</t>
   </si>
   <si>
-    <t>Lidah Kucing Coklat</t>
-  </si>
-  <si>
     <t>Lidah Kucing Keju</t>
   </si>
   <si>
-    <t>Lidah Kucing Choco</t>
-  </si>
-  <si>
     <t>Sagu Pandan</t>
   </si>
   <si>
-    <t>Sagu Coklat</t>
-  </si>
-  <si>
     <t>Choco Cheese</t>
   </si>
   <si>
@@ -104,12 +95,6 @@
     <t>Nastar Garis</t>
   </si>
   <si>
-    <t>Santa Claus Bag</t>
-  </si>
-  <si>
-    <t>Red Box</t>
-  </si>
-  <si>
     <t>Round Bag</t>
   </si>
   <si>
@@ -176,31 +161,19 @@
     <t>Nastar Box</t>
   </si>
   <si>
-    <t>Mieting Keju</t>
-  </si>
-  <si>
-    <t>Mieting Pedas</t>
-  </si>
-  <si>
     <t>Almond Disc Original</t>
   </si>
   <si>
     <t>Almond Disc Coklat</t>
   </si>
   <si>
-    <t>Almond Disc Mocca</t>
-  </si>
-  <si>
-    <t>Almond Disc Green Tea</t>
-  </si>
-  <si>
-    <t>Almond Disc Cheese</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>???</t>
+    <t>Double Choco</t>
+  </si>
+  <si>
+    <t>Crunchy Cashew</t>
+  </si>
+  <si>
+    <t>Half Price</t>
   </si>
 </sst>
 </file>
@@ -658,40 +631,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="19" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="2" max="3" width="19" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>78000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="2">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -699,7 +678,7 @@
         <v>78000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -707,7 +686,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -715,156 +694,169 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>73000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="2">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>115000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>62000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>62000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
         <v>73000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>730000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
-        <v>115000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B13" s="2">
+        <v>86000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>73000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>730000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>86000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>48000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>73000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="2">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <v>55000</v>
+      </c>
+      <c r="C19" s="2">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
         <v>60000</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2">
-        <v>48000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="C20" s="2">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2">
-        <v>48000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
       <c r="B21" s="2">
-        <v>48000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>78000</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2">
-        <v>60000</v>
+        <v>78000</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44000</v>
       </c>
     </row>
   </sheetData>
@@ -877,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,7 +894,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2">
         <v>150000</v>
@@ -910,7 +902,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>180000</v>
@@ -918,7 +910,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>205000</v>
@@ -926,7 +918,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2">
         <v>265000</v>
@@ -934,7 +926,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2">
         <v>340000</v>
@@ -942,7 +934,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>440000</v>
@@ -950,7 +942,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>540000</v>
@@ -958,7 +950,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>640000</v>
@@ -966,7 +958,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2">
         <v>620000</v>
@@ -974,7 +966,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2">
         <v>720000</v>
@@ -982,7 +974,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2">
         <v>920000</v>
@@ -990,7 +982,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
         <v>730000</v>
@@ -998,7 +990,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
         <v>930000</v>
@@ -1006,7 +998,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2">
         <v>1130000</v>
@@ -1014,7 +1006,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2">
         <v>400000</v>
@@ -1022,7 +1014,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2">
         <v>500000</v>
@@ -1030,7 +1022,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2">
         <v>210000</v>
@@ -1038,7 +1030,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="2">
         <v>330000</v>
@@ -1051,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,7 +1070,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2">
         <v>21000</v>
@@ -1086,7 +1078,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2">
         <v>29000</v>
@@ -1094,7 +1086,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2">
         <v>29000</v>
@@ -1102,7 +1094,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
         <v>29000</v>
@@ -1110,58 +1102,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
-        <v>29000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="2">
         <v>40000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="2">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="2">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="2">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="2">
-        <v>45000</v>
       </c>
     </row>
   </sheetData>
@@ -1171,332 +1123,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33.81640625" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>8762</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>8794</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>8800</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44">
-        <v>8778</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>